<commit_message>
delete space and indention in input mode
</commit_message>
<xml_diff>
--- a/benchmark/ffo_history.xlsx
+++ b/benchmark/ffo_history.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\github\othello\Egaroucid\benchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36C126AB-937E-4EB8-BA1E-6116F6CD106E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C4F5591-BB66-4E88-B30B-78D5A64240C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="48540" yWindow="3528" windowWidth="34560" windowHeight="18600" activeTab="1" xr2:uid="{1ECBFA7D-B1B2-4BC3-8930-4A242FE14EB6}"/>
+    <workbookView xWindow="50880" yWindow="3048" windowWidth="34560" windowHeight="18540" xr2:uid="{1ECBFA7D-B1B2-4BC3-8930-4A242FE14EB6}"/>
   </bookViews>
   <sheets>
     <sheet name="core i9 13900k" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t>5.4.1</t>
     <phoneticPr fontId="1"/>
@@ -106,6 +106,10 @@
   </si>
   <si>
     <t>Core i9 11900K</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>6.4.0</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -308,9 +312,18 @@
             <c:strRef>
               <c:f>'core i9 13900k'!$A$2:$A$37</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
+                  <c:v>6.1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>6.3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.4.0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -322,7 +335,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>80.251999999999995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>71.456999999999994</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>47.935000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>35.506999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -638,9 +660,18 @@
             <c:strRef>
               <c:f>'core i9 13900k'!$A$2:$A$37</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
+                  <c:v>6.1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>6.3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.4.0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -652,7 +683,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>40280448340</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30186743066</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>24847574333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>26310910398</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -968,9 +1008,18 @@
             <c:strRef>
               <c:f>'core i9 13900k'!$A$2:$A$37</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
+                  <c:v>6.1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>6.3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.4.0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -982,7 +1031,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>501924541</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>422446269</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>518359744</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>741006291</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6101,11 +6159,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07F9F6D2-0DD9-4DE9-BCD9-C5D71918CFAE}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S26" sqref="S26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="3" max="3" width="12.59765625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
@@ -6126,32 +6187,59 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B2">
-        <v>47.935000000000002</v>
+        <v>80.251999999999995</v>
       </c>
       <c r="C2">
-        <v>24847574333</v>
+        <v>40280448340</v>
       </c>
       <c r="D2">
-        <v>518359744</v>
+        <v>501924541</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3">
+        <v>71.456999999999994</v>
+      </c>
+      <c r="C3">
+        <v>30186743066</v>
+      </c>
+      <c r="D3">
+        <v>422446269</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <v>47.935000000000002</v>
+      </c>
+      <c r="C4">
+        <v>24847574333</v>
+      </c>
+      <c r="D4">
+        <v>518359744</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1">
+        <v>35.506999999999998</v>
+      </c>
+      <c r="C5">
+        <v>26310910398</v>
+      </c>
+      <c r="D5">
+        <v>741006291</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B6" s="1"/>
@@ -6187,8 +6275,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{387CFE65-7368-4EDF-98B2-6FDEFECB003E}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R10" sqref="R10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
update benchmark and web resources
</commit_message>
<xml_diff>
--- a/benchmark/ffo_history.xlsx
+++ b/benchmark/ffo_history.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\github\othello\Egaroucid\benchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B45DA523-439F-43FE-95CA-8B7FAB5B733B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D54AB0F6-769C-4164-AE80-EFD42A69623B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="46896" yWindow="6588" windowWidth="34560" windowHeight="18540" xr2:uid="{1ECBFA7D-B1B2-4BC3-8930-4A242FE14EB6}"/>
+    <workbookView xWindow="49908" yWindow="3780" windowWidth="34560" windowHeight="18600" xr2:uid="{1ECBFA7D-B1B2-4BC3-8930-4A242FE14EB6}"/>
   </bookViews>
   <sheets>
     <sheet name="core i9 13900k" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
   <si>
     <t>5.4.1</t>
     <phoneticPr fontId="1"/>
@@ -110,6 +110,10 @@
   </si>
   <si>
     <t>6.4.0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>6.5.0</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -312,7 +316,7 @@
             <c:strRef>
               <c:f>'core i9 13900k'!$A$2:$A$37</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>6.1.0</c:v>
                 </c:pt>
@@ -324,16 +328,19 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>6.4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.5.0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'core i9 13900k'!$B$2:$B$5</c:f>
+              <c:f>'core i9 13900k'!$B$2:$B$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>80.251999999999995</c:v>
                 </c:pt>
@@ -345,6 +352,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>36.085999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>35.334000000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -660,7 +670,7 @@
             <c:strRef>
               <c:f>'core i9 13900k'!$A$2:$A$37</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>6.1.0</c:v>
                 </c:pt>
@@ -672,16 +682,19 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>6.4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.5.0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'core i9 13900k'!$C$2:$C$5</c:f>
+              <c:f>'core i9 13900k'!$C$2:$C$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>40280448340</c:v>
                 </c:pt>
@@ -693,6 +706,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>25881299806</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25787196363</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1008,7 +1024,7 @@
             <c:strRef>
               <c:f>'core i9 13900k'!$A$2:$A$37</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>6.1.0</c:v>
                 </c:pt>
@@ -1020,16 +1036,19 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>6.4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.5.0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'core i9 13900k'!$D$2:$D$5</c:f>
+              <c:f>'core i9 13900k'!$D$2:$D$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>501924541</c:v>
                 </c:pt>
@@ -1041,6 +1060,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>717211655</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>729812542</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6160,7 +6182,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="R22" sqref="R22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
@@ -6242,9 +6264,18 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="1">
+        <v>35.334000000000003</v>
+      </c>
+      <c r="C6" s="1">
+        <v>25787196363</v>
+      </c>
+      <c r="D6" s="1">
+        <v>729812542</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B7" s="1"/>

</xml_diff>

<commit_message>
add egaroucid 6.0.X ffotest
</commit_message>
<xml_diff>
--- a/benchmark/ffo_history.xlsx
+++ b/benchmark/ffo_history.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\github\othello\Egaroucid\benchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD822FBA-4AD0-4F64-BBBD-C136F858414B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48E4EC76-0D25-4B3A-90BF-DBEC796597F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="49908" yWindow="3780" windowWidth="34560" windowHeight="18600" xr2:uid="{1ECBFA7D-B1B2-4BC3-8930-4A242FE14EB6}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="34560" windowHeight="18600" xr2:uid="{1ECBFA7D-B1B2-4BC3-8930-4A242FE14EB6}"/>
   </bookViews>
   <sheets>
     <sheet name="core i9 13900k" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
   <si>
     <t>5.4.1</t>
     <phoneticPr fontId="1"/>
@@ -114,6 +114,10 @@
   </si>
   <si>
     <t>6.5.0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>7.0.0</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -314,46 +318,55 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'core i9 13900k'!$A$2:$A$37</c:f>
+              <c:f>'core i9 13900k'!$A$2:$A$36</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>6.0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>6.1.0</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>6.2.0</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>6.3.0</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>6.4.0</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>6.5.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0.0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'core i9 13900k'!$B$2:$B$6</c:f>
+              <c:f>'core i9 13900k'!$B$2:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>105.497</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>80.251999999999995</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>71.456999999999994</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>47.935000000000002</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>36.085999999999999</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>34.901000000000003</c:v>
                 </c:pt>
               </c:numCache>
@@ -668,46 +681,55 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'core i9 13900k'!$A$2:$A$37</c:f>
+              <c:f>'core i9 13900k'!$A$2:$A$36</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>6.0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>6.1.0</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>6.2.0</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>6.3.0</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>6.4.0</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>6.5.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0.0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'core i9 13900k'!$C$2:$C$6</c:f>
+              <c:f>'core i9 13900k'!$C$2:$C$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>45030833773</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>40280448340</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>30186743066</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>24847574333</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>25881299806</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>25129728758</c:v>
                 </c:pt>
               </c:numCache>
@@ -1022,46 +1044,55 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'core i9 13900k'!$A$2:$A$37</c:f>
+              <c:f>'core i9 13900k'!$A$2:$A$36</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>6.0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>6.1.0</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>6.2.0</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>6.3.0</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>6.4.0</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>6.5.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0.0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'core i9 13900k'!$D$2:$D$6</c:f>
+              <c:f>'core i9 13900k'!$D$2:$D$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>426844685.37493902</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>501924541</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>422446269</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>518359744</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>717211655</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>720028903</c:v>
                 </c:pt>
               </c:numCache>
@@ -5883,9 +5914,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 テーマ">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -5923,7 +5954,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -6029,7 +6060,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -6171,7 +6202,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -6182,7 +6213,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="S12" sqref="S12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
@@ -6209,80 +6240,92 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2">
-        <v>80.251999999999995</v>
+        <v>105.497</v>
       </c>
       <c r="C2">
-        <v>40280448340</v>
+        <v>45030833773</v>
       </c>
       <c r="D2">
-        <v>501924541</v>
+        <v>426844685.37493902</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3">
-        <v>71.456999999999994</v>
+        <v>80.251999999999995</v>
       </c>
       <c r="C3">
-        <v>30186743066</v>
+        <v>40280448340</v>
       </c>
       <c r="D3">
-        <v>422446269</v>
+        <v>501924541</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4">
-        <v>47.935000000000002</v>
+        <v>71.456999999999994</v>
       </c>
       <c r="C4">
-        <v>24847574333</v>
+        <v>30186743066</v>
       </c>
       <c r="D4">
-        <v>518359744</v>
+        <v>422446269</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="1">
-        <v>36.085999999999999</v>
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>47.935000000000002</v>
       </c>
       <c r="C5">
-        <v>25881299806</v>
+        <v>24847574333</v>
       </c>
       <c r="D5">
-        <v>717211655</v>
+        <v>518359744</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1">
-        <v>34.901000000000003</v>
-      </c>
-      <c r="C6" s="1">
-        <v>25129728758</v>
-      </c>
-      <c r="D6" s="1">
-        <v>720028903</v>
+        <v>36.085999999999999</v>
+      </c>
+      <c r="C6">
+        <v>25881299806</v>
+      </c>
+      <c r="D6">
+        <v>717211655</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="1">
+        <v>34.901000000000003</v>
+      </c>
+      <c r="C7" s="1">
+        <v>25129728758</v>
+      </c>
+      <c r="D7" s="1">
+        <v>720028903</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>

</xml_diff>

<commit_message>
update ffo history, #229
</commit_message>
<xml_diff>
--- a/benchmark/ffo_history.xlsx
+++ b/benchmark/ffo_history.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\github\othello\Egaroucid\benchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B2B8DD6-D982-400A-BC9B-9BE7D6BA32F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA91213-3AD8-4A47-A801-0A9B407DB7F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6828" yWindow="2784" windowWidth="18228" windowHeight="18600" xr2:uid="{1ECBFA7D-B1B2-4BC3-8930-4A242FE14EB6}"/>
+    <workbookView xWindow="49368" yWindow="6420" windowWidth="34560" windowHeight="18600" xr2:uid="{1ECBFA7D-B1B2-4BC3-8930-4A242FE14EB6}"/>
   </bookViews>
   <sheets>
     <sheet name="core i9 13900k" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
   <si>
     <t>5.4.1</t>
     <phoneticPr fontId="1"/>
@@ -118,6 +118,10 @@
   </si>
   <si>
     <t>7.0.0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>7.1.0</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -320,7 +324,7 @@
             <c:strRef>
               <c:f>'core i9 13900k'!$A$2:$A$36</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>6.0.0</c:v>
                 </c:pt>
@@ -341,16 +345,19 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>7.0.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.1.0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'core i9 13900k'!$B$2:$B$8</c:f>
+              <c:f>'core i9 13900k'!$B$2:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>105.497</c:v>
                 </c:pt>
@@ -371,6 +378,9 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>28.722000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>27.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -742,7 +752,7 @@
             <c:strRef>
               <c:f>'core i9 13900k'!$A$2:$A$36</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>6.0.0</c:v>
                 </c:pt>
@@ -763,16 +773,19 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>7.0.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.1.0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'core i9 13900k'!$C$2:$C$8</c:f>
+              <c:f>'core i9 13900k'!$C$2:$C$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>45030833773</c:v>
                 </c:pt>
@@ -793,6 +806,9 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>25883018262</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25746866156</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1164,7 +1180,7 @@
             <c:strRef>
               <c:f>'core i9 13900k'!$A$2:$A$36</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>6.0.0</c:v>
                 </c:pt>
@@ -1185,16 +1201,19 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>7.0.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.1.0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'core i9 13900k'!$D$2:$D$8</c:f>
+              <c:f>'core i9 13900k'!$D$2:$D$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>426844685.37493902</c:v>
                 </c:pt>
@@ -1215,6 +1234,9 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>901156544</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>927814996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6390,7 +6412,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
@@ -6514,9 +6536,18 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="1">
+        <v>27.75</v>
+      </c>
+      <c r="C9" s="1">
+        <v>25746866156</v>
+      </c>
+      <c r="D9" s="1">
+        <v>927814996</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B11" s="1"/>

</xml_diff>

<commit_message>
update ffo test graph
</commit_message>
<xml_diff>
--- a/benchmark/ffo_history.xlsx
+++ b/benchmark/ffo_history.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\github\othello\Egaroucid\benchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA91213-3AD8-4A47-A801-0A9B407DB7F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E48FD2-57C5-45FB-B623-E5C0B0A4553F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="49368" yWindow="6420" windowWidth="34560" windowHeight="18600" xr2:uid="{1ECBFA7D-B1B2-4BC3-8930-4A242FE14EB6}"/>
+    <workbookView xWindow="43190" yWindow="2390" windowWidth="28800" windowHeight="15370" xr2:uid="{1ECBFA7D-B1B2-4BC3-8930-4A242FE14EB6}"/>
   </bookViews>
   <sheets>
     <sheet name="core i9 13900k" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
   <si>
     <t>5.4.1</t>
     <phoneticPr fontId="1"/>
@@ -122,6 +122,10 @@
   </si>
   <si>
     <t>7.1.0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>7.2.0</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -324,7 +328,7 @@
             <c:strRef>
               <c:f>'core i9 13900k'!$A$2:$A$36</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>6.0.0</c:v>
                 </c:pt>
@@ -348,16 +352,19 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>7.1.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.2.0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'core i9 13900k'!$B$2:$B$9</c:f>
+              <c:f>'core i9 13900k'!$B$2:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>105.497</c:v>
                 </c:pt>
@@ -381,6 +388,9 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>27.75</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>27.364000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -752,7 +762,7 @@
             <c:strRef>
               <c:f>'core i9 13900k'!$A$2:$A$36</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>6.0.0</c:v>
                 </c:pt>
@@ -776,16 +786,19 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>7.1.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.2.0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'core i9 13900k'!$C$2:$C$9</c:f>
+              <c:f>'core i9 13900k'!$C$2:$C$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>45030833773</c:v>
                 </c:pt>
@@ -809,6 +822,9 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>25746866156</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>26421069847</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1180,7 +1196,7 @@
             <c:strRef>
               <c:f>'core i9 13900k'!$A$2:$A$36</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>6.0.0</c:v>
                 </c:pt>
@@ -1204,16 +1220,19 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>7.1.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.2.0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'core i9 13900k'!$D$2:$D$9</c:f>
+              <c:f>'core i9 13900k'!$D$2:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>426844685.37493902</c:v>
                 </c:pt>
@@ -1237,6 +1256,9 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>927814996</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>965541216</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6412,15 +6434,15 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="S23" sqref="S23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="3" max="3" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.58203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -6437,7 +6459,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -6451,7 +6473,7 @@
         <v>426844685.37493902</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -6465,7 +6487,7 @@
         <v>501924541</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -6479,7 +6501,7 @@
         <v>422446269</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -6493,7 +6515,7 @@
         <v>518359744</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -6507,7 +6529,7 @@
         <v>717211655</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -6521,7 +6543,7 @@
         <v>720028903</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -6535,7 +6557,7 @@
         <v>901156544</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -6549,7 +6571,21 @@
         <v>927814996</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10">
+        <v>27.364000000000001</v>
+      </c>
+      <c r="C10">
+        <v>26421069847</v>
+      </c>
+      <c r="D10">
+        <v>965541216</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="1"/>
     </row>
   </sheetData>
@@ -6567,9 +6603,9 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -6586,7 +6622,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -6600,7 +6636,7 @@
         <v>95653834</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -6614,7 +6650,7 @@
         <v>174800705</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -6628,7 +6664,7 @@
         <v>155858072</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -6642,7 +6678,7 @@
         <v>128218350</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -6656,7 +6692,7 @@
         <v>161328242</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -6670,7 +6706,7 @@
         <v>176829434</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -6684,7 +6720,7 @@
         <v>247393374</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -6698,7 +6734,7 @@
         <v>271332246</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -6712,7 +6748,7 @@
         <v>273481086</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
update ffo history for 7.4.0
</commit_message>
<xml_diff>
--- a/benchmark/ffo_history.xlsx
+++ b/benchmark/ffo_history.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\github\othello\Egaroucid\benchmark\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\egaroucid\Egaroucid\benchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02DF7DD0-8323-4B0A-93C0-0560947579F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74669A61-F9B0-4647-A3A9-DE66E66B37CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38340" yWindow="4200" windowWidth="17490" windowHeight="15370" xr2:uid="{1ECBFA7D-B1B2-4BC3-8930-4A242FE14EB6}"/>
+    <workbookView xWindow="2868" yWindow="3024" windowWidth="18432" windowHeight="16404" xr2:uid="{1ECBFA7D-B1B2-4BC3-8930-4A242FE14EB6}"/>
   </bookViews>
   <sheets>
     <sheet name="core i9 13900k" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
   <si>
     <t>5.4.1</t>
     <phoneticPr fontId="1"/>
@@ -130,6 +130,10 @@
   </si>
   <si>
     <t>7.3.0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>7.4.0</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -332,7 +336,7 @@
             <c:strRef>
               <c:f>'core i9 13900k'!$A$2:$A$36</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>6.0.0</c:v>
                 </c:pt>
@@ -362,16 +366,19 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>7.3.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7.4.0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'core i9 13900k'!$B$2:$B$11</c:f>
+              <c:f>'core i9 13900k'!$B$2:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>105.497</c:v>
                 </c:pt>
@@ -401,6 +408,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>22.891999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>23.303000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -772,7 +782,7 @@
             <c:strRef>
               <c:f>'core i9 13900k'!$A$2:$A$36</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>6.0.0</c:v>
                 </c:pt>
@@ -802,16 +812,19 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>7.3.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7.4.0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'core i9 13900k'!$C$2:$C$11</c:f>
+              <c:f>'core i9 13900k'!$C$2:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>45030833773</c:v>
                 </c:pt>
@@ -841,6 +854,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>19272934563</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>17784812781</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1212,7 +1228,7 @@
             <c:strRef>
               <c:f>'core i9 13900k'!$A$2:$A$36</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>6.0.0</c:v>
                 </c:pt>
@@ -1242,16 +1258,19 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>7.3.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7.4.0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'core i9 13900k'!$D$2:$D$11</c:f>
+              <c:f>'core i9 13900k'!$D$2:$D$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>426844685.37493902</c:v>
                 </c:pt>
@@ -1281,6 +1300,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>841906978</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>763198419</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6453,18 +6475,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07F9F6D2-0DD9-4DE9-BCD9-C5D71918CFAE}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="T27" sqref="T27"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="12.58203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -6481,7 +6503,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -6495,7 +6517,7 @@
         <v>426844685.37493902</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -6509,7 +6531,7 @@
         <v>501924541</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -6523,7 +6545,7 @@
         <v>422446269</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -6537,7 +6559,7 @@
         <v>518359744</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -6551,7 +6573,7 @@
         <v>717211655</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -6565,7 +6587,7 @@
         <v>720028903</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -6579,7 +6601,7 @@
         <v>901156544</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -6593,7 +6615,7 @@
         <v>927814996</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -6607,7 +6629,7 @@
         <v>965541216</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -6619,6 +6641,20 @@
       </c>
       <c r="D11">
         <v>841906978</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="1">
+        <v>23.303000000000001</v>
+      </c>
+      <c r="C12">
+        <v>17784812781</v>
+      </c>
+      <c r="D12">
+        <v>763198419</v>
       </c>
     </row>
   </sheetData>
@@ -6636,9 +6672,9 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -6655,7 +6691,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -6669,7 +6705,7 @@
         <v>95653834</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -6683,7 +6719,7 @@
         <v>174800705</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -6697,7 +6733,7 @@
         <v>155858072</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -6711,7 +6747,7 @@
         <v>128218350</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -6725,7 +6761,7 @@
         <v>161328242</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -6739,7 +6775,7 @@
         <v>176829434</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -6753,7 +6789,7 @@
         <v>247393374</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -6767,7 +6803,7 @@
         <v>271332246</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -6781,7 +6817,7 @@
         <v>273481086</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>13</v>
       </c>

</xml_diff>